<commit_message>
Several fixes and adjustements for the validator
</commit_message>
<xml_diff>
--- a/templates/TemplateColumns2Models_v5a.xlsx
+++ b/templates/TemplateColumns2Models_v5a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lg10/Workspace/git/fork/PGS_template_validator/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B128D6A4-1DA8-E643-A093-D48F24BB9386}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C70414-DF2D-724D-836A-8FC733C0AD2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31480" yWindow="2180" windowWidth="28800" windowHeight="15200" xr2:uid="{B0CC4535-7E6E-584E-9FDE-AD77876CF244}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="150">
   <si>
     <t>Sheet</t>
   </si>
@@ -1084,9 +1084,6 @@
     <t>Must be linked by object (PSS)</t>
   </si>
   <si>
-    <t>Must be linked by object (Cohort)</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -1118,6 +1115,9 @@
   </si>
   <si>
     <t>sampleset</t>
+  </si>
+  <si>
+    <t>Must be linked by object (Cohort) - only mandatory for Sample Testing</t>
   </si>
 </sst>
 </file>
@@ -2025,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FDEE91-4AEE-FD49-8B2B-E0D2B4B6944F}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2053,10 +2053,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>140</v>
       </c>
       <c r="G1" s="30" t="s">
         <v>56</v>
@@ -2076,7 +2076,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="31"/>
     </row>
@@ -2094,10 +2094,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2114,10 +2114,10 @@
         <v>45</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2177,10 +2177,10 @@
         <v>47</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2197,10 +2197,10 @@
         <v>48</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2217,7 +2217,7 @@
         <v>50</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="31"/>
     </row>
@@ -2235,10 +2235,10 @@
         <v>49</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2255,10 +2255,10 @@
         <v>51</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2275,7 +2275,7 @@
         <v>52</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F13" s="31"/>
     </row>
@@ -2293,7 +2293,7 @@
         <v>90</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F14" s="31"/>
     </row>
@@ -2311,10 +2311,10 @@
         <v>53</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="27" customHeight="1">
@@ -2331,7 +2331,7 @@
         <v>54</v>
       </c>
       <c r="E16" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F16" s="46"/>
       <c r="G16" s="47"/>
@@ -2347,10 +2347,10 @@
         <v>55</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="4" t="s">
@@ -2368,13 +2368,13 @@
         <v>55</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>59</v>
@@ -2391,10 +2391,10 @@
         <v>55</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="4" t="s">
@@ -2415,7 +2415,7 @@
         <v>60</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" s="31"/>
     </row>
@@ -2433,7 +2433,7 @@
         <v>61</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F21" s="31"/>
     </row>
@@ -2451,10 +2451,10 @@
         <v>62</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2471,7 +2471,7 @@
         <v>63</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" s="31"/>
     </row>
@@ -2489,7 +2489,7 @@
         <v>64</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="31"/>
     </row>
@@ -2507,7 +2507,7 @@
         <v>65</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" s="31"/>
     </row>
@@ -2525,7 +2525,7 @@
         <v>134</v>
       </c>
       <c r="E26" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" s="31"/>
       <c r="G26" s="3" t="s">
@@ -2546,10 +2546,10 @@
         <v>66</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2566,7 +2566,7 @@
         <v>67</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" s="31"/>
     </row>
@@ -2584,7 +2584,7 @@
         <v>68</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="31"/>
     </row>
@@ -2602,7 +2602,7 @@
         <v>69</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" s="31"/>
     </row>
@@ -2620,7 +2620,7 @@
         <v>87</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F31" s="31"/>
     </row>
@@ -2638,7 +2638,7 @@
         <v>133</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F32" s="31"/>
       <c r="G32" s="3" t="s">
@@ -2659,13 +2659,11 @@
         <v>71</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="F33" s="31" t="s">
         <v>141</v>
       </c>
+      <c r="F33" s="31"/>
       <c r="G33" s="3" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1">
@@ -2682,7 +2680,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" s="46"/>
       <c r="G34" s="47"/>
@@ -2698,13 +2696,13 @@
         <v>72</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>136</v>
@@ -2721,13 +2719,13 @@
         <v>72</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>137</v>
@@ -2747,10 +2745,10 @@
         <v>130</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="27" customHeight="1" thickBot="1">
@@ -2879,7 +2877,7 @@
         <v>81</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F45" s="31"/>
     </row>
@@ -2897,7 +2895,7 @@
         <v>82</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F46" s="46"/>
       <c r="G46" s="47"/>
@@ -2916,10 +2914,10 @@
         <v>73</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="27" customHeight="1">
@@ -2936,7 +2934,7 @@
         <v>75</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F48" s="46"/>
       <c r="G48" s="47"/>

</xml_diff>